<commit_message>
Change xsl file with books information
</commit_message>
<xml_diff>
--- a/disk-archive-data/xls/Books.xlsx
+++ b/disk-archive-data/xls/Books.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="71">
   <si>
     <t>Мигель де Сервантес Сааведра</t>
   </si>
@@ -210,13 +210,25 @@
     <t>Поэзия</t>
   </si>
   <si>
-    <t>Год издания (начало)</t>
-  </si>
-  <si>
-    <t>Год издания (завершение)</t>
-  </si>
-  <si>
     <t>Украинский Советский Энциклопедический словарь</t>
+  </si>
+  <si>
+    <t>Ф.С. Бабичев, Р.И. Вишневский, И.А. Дзеверин, М.П. Зяблюк, Ю.Ю. Кондуфор, А.В. Кудрицкий, А.М. Лопухов, И.И. Лукинов, А.М. Маринич, А.П. Ромоданов, А.И. Троян</t>
+  </si>
+  <si>
+    <t>Ф.С. Бабичев, Р.И. Вишневский, И.А. Дзеверин, М.П. Зяблюк, Ю.Ю. Кондуфор, А.В. Кудрицкий, А.М. Лопухов, И.И. Лукинов, А.М. Маринич, А.П. Ромоданов</t>
+  </si>
+  <si>
+    <t>Год издания</t>
+  </si>
+  <si>
+    <t>Количество томов в год</t>
+  </si>
+  <si>
+    <t>38A</t>
+  </si>
+  <si>
+    <t>Том (старая маркировка)</t>
   </si>
 </sst>
 </file>
@@ -556,10 +568,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F179"/>
+  <dimension ref="A1:G179"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A156" workbookViewId="0">
-      <selection activeCell="B180" sqref="B180"/>
+    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
+      <selection activeCell="D163" sqref="D163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -568,10 +580,11 @@
     <col min="2" max="2" width="49.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -585,13 +598,16 @@
         <v>5</v>
       </c>
       <c r="E1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="F1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="G1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -608,7 +624,7 @@
         <v>1979</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -625,7 +641,7 @@
         <v>1979</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -642,7 +658,7 @@
         <v>1981</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -659,7 +675,7 @@
         <v>1981</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -676,7 +692,7 @@
         <v>1981</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -693,7 +709,7 @@
         <v>1975</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -710,7 +726,7 @@
         <v>1975</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -727,7 +743,7 @@
         <v>1975</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -744,7 +760,7 @@
         <v>1981</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -761,7 +777,7 @@
         <v>1981</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -778,7 +794,7 @@
         <v>1981</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -795,7 +811,7 @@
         <v>1988</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -812,7 +828,7 @@
         <v>1988</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -829,7 +845,7 @@
         <v>1988</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -1094,6 +1110,9 @@
       <c r="C31">
         <v>2</v>
       </c>
+      <c r="D31">
+        <v>7</v>
+      </c>
       <c r="E31">
         <v>1978</v>
       </c>
@@ -1108,6 +1127,9 @@
       <c r="C32">
         <v>3</v>
       </c>
+      <c r="D32">
+        <v>7</v>
+      </c>
       <c r="E32">
         <v>1978</v>
       </c>
@@ -1122,6 +1144,9 @@
       <c r="C33">
         <v>4</v>
       </c>
+      <c r="D33">
+        <v>7</v>
+      </c>
       <c r="E33">
         <v>1978</v>
       </c>
@@ -1136,6 +1161,9 @@
       <c r="C34">
         <v>5</v>
       </c>
+      <c r="D34">
+        <v>7</v>
+      </c>
       <c r="E34">
         <v>1978</v>
       </c>
@@ -1150,6 +1178,9 @@
       <c r="C35">
         <v>6</v>
       </c>
+      <c r="D35">
+        <v>7</v>
+      </c>
       <c r="E35">
         <v>1978</v>
       </c>
@@ -1164,6 +1195,9 @@
       <c r="C36">
         <v>7</v>
       </c>
+      <c r="D36">
+        <v>7</v>
+      </c>
       <c r="E36">
         <v>1978</v>
       </c>
@@ -3004,7 +3038,7 @@
         <v>1976</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>39</v>
       </c>
@@ -3021,7 +3055,7 @@
         <v>1976</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>39</v>
       </c>
@@ -3038,7 +3072,7 @@
         <v>1976</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>39</v>
       </c>
@@ -3055,7 +3089,7 @@
         <v>1976</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>39</v>
       </c>
@@ -3072,7 +3106,7 @@
         <v>1976</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>40</v>
       </c>
@@ -3089,7 +3123,7 @@
         <v>1975</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>40</v>
       </c>
@@ -3106,7 +3140,7 @@
         <v>1975</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>40</v>
       </c>
@@ -3123,7 +3157,7 @@
         <v>1975</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>40</v>
       </c>
@@ -3140,7 +3174,7 @@
         <v>1975</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>40</v>
       </c>
@@ -3157,7 +3191,7 @@
         <v>1975</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>40</v>
       </c>
@@ -3174,7 +3208,7 @@
         <v>1975</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>40</v>
       </c>
@@ -3191,7 +3225,7 @@
         <v>1975</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>40</v>
       </c>
@@ -3208,7 +3242,7 @@
         <v>1975</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>42</v>
       </c>
@@ -3216,13 +3250,22 @@
         <v>41</v>
       </c>
       <c r="C157">
-        <v>4</v>
+        <v>7</v>
+      </c>
+      <c r="D157">
+        <v>86</v>
       </c>
       <c r="E157">
         <v>1891</v>
       </c>
-    </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F157">
+        <v>4</v>
+      </c>
+      <c r="G157">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>42</v>
       </c>
@@ -3230,13 +3273,22 @@
         <v>41</v>
       </c>
       <c r="C158">
-        <v>11</v>
+        <v>21</v>
+      </c>
+      <c r="D158">
+        <v>86</v>
       </c>
       <c r="E158">
         <v>1893</v>
       </c>
-    </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F158">
+        <v>11</v>
+      </c>
+      <c r="G158">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>42</v>
       </c>
@@ -3244,13 +3296,22 @@
         <v>41</v>
       </c>
       <c r="C159">
-        <v>34</v>
+        <v>45</v>
+      </c>
+      <c r="D159">
+        <v>86</v>
       </c>
       <c r="E159">
-        <v>1902</v>
-      </c>
-    </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1898</v>
+      </c>
+      <c r="F159">
+        <v>23</v>
+      </c>
+      <c r="G159">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>42</v>
       </c>
@@ -3258,10 +3319,22 @@
         <v>41</v>
       </c>
       <c r="C160">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="D160">
+        <v>86</v>
+      </c>
+      <c r="E160">
+        <v>1900</v>
+      </c>
+      <c r="F160">
+        <v>29</v>
+      </c>
+      <c r="G160">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>42</v>
       </c>
@@ -3269,13 +3342,22 @@
         <v>41</v>
       </c>
       <c r="C161">
-        <v>57</v>
+        <v>67</v>
+      </c>
+      <c r="D161">
+        <v>86</v>
       </c>
       <c r="E161">
-        <v>1900</v>
-      </c>
-    </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1901</v>
+      </c>
+      <c r="F161">
+        <v>34</v>
+      </c>
+      <c r="G161">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>42</v>
       </c>
@@ -3285,11 +3367,20 @@
       <c r="C162">
         <v>71</v>
       </c>
+      <c r="D162">
+        <v>86</v>
+      </c>
       <c r="E162">
         <v>1902</v>
       </c>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F162">
+        <v>36</v>
+      </c>
+      <c r="G162">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>42</v>
       </c>
@@ -3299,11 +3390,20 @@
       <c r="C163">
         <v>76</v>
       </c>
+      <c r="D163">
+        <v>86</v>
+      </c>
       <c r="E163">
         <v>1903</v>
       </c>
-    </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F163" t="s">
+        <v>69</v>
+      </c>
+      <c r="G163">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>44</v>
       </c>
@@ -3320,7 +3420,7 @@
         <v>1977</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>45</v>
       </c>
@@ -3337,7 +3437,7 @@
         <v>1978</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>47</v>
       </c>
@@ -3354,7 +3454,7 @@
         <v>1977</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>48</v>
       </c>
@@ -3365,7 +3465,7 @@
         <v>1979</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>48</v>
       </c>
@@ -3382,7 +3482,7 @@
         <v>1976</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>48</v>
       </c>
@@ -3399,7 +3499,7 @@
         <v>1976</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>50</v>
       </c>
@@ -3410,7 +3510,7 @@
         <v>1990</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>53</v>
       </c>
@@ -3421,7 +3521,7 @@
         <v>1988</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>55</v>
       </c>
@@ -3432,7 +3532,7 @@
         <v>1990</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>57</v>
       </c>
@@ -3443,7 +3543,7 @@
         <v>1988</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>59</v>
       </c>
@@ -3454,7 +3554,7 @@
         <v>1991</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B175" t="s">
         <v>61</v>
       </c>
@@ -3462,7 +3562,7 @@
         <v>1988</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>62</v>
       </c>
@@ -3473,9 +3573,12 @@
         <v>1988</v>
       </c>
     </row>
-    <row r="177" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>65</v>
+      </c>
       <c r="B177" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C177">
         <v>1</v>
@@ -3484,15 +3587,15 @@
         <v>3</v>
       </c>
       <c r="E177">
-        <v>1986</v>
-      </c>
-      <c r="F177">
         <v>1988</v>
       </c>
     </row>
-    <row r="178" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>66</v>
+      </c>
       <c r="B178" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C178">
         <v>2</v>
@@ -3501,15 +3604,15 @@
         <v>3</v>
       </c>
       <c r="E178">
-        <v>1986</v>
-      </c>
-      <c r="F178">
         <v>1988</v>
       </c>
     </row>
-    <row r="179" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>66</v>
+      </c>
       <c r="B179" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C179">
         <v>3</v>
@@ -3518,9 +3621,6 @@
         <v>3</v>
       </c>
       <c r="E179">
-        <v>1986</v>
-      </c>
-      <c r="F179">
         <v>1988</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated jetty/Switched from csvUploadStrategy to xlsUploadStrategy/Fix tests
</commit_message>
<xml_diff>
--- a/disk-archive-data/xls/Books.xlsx
+++ b/disk-archive-data/xls/Books.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\disk-archive\disk-archive-data\xls\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585"/>
   </bookViews>
@@ -11,7 +16,7 @@
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621" refMode="R1C1"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -272,7 +277,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -280,14 +285,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -325,9 +333,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -362,7 +370,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -397,7 +405,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -573,8 +581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H179"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A137" workbookViewId="0">
-      <selection activeCell="G162" sqref="G162"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1560,7 +1568,7 @@
         <v>3</v>
       </c>
       <c r="D57">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E57">
         <v>1981</v>
@@ -1577,7 +1585,7 @@
         <v>4</v>
       </c>
       <c r="D58">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E58">
         <v>1981</v>
@@ -1594,7 +1602,7 @@
         <v>5</v>
       </c>
       <c r="D59">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E59">
         <v>1981</v>

</xml_diff>

<commit_message>
BOOK-16: implementation of job logic and fix of old classes what were involved into book saving process.
</commit_message>
<xml_diff>
--- a/disk-archive-data/xls/Books.xlsx
+++ b/disk-archive-data/xls/Books.xlsx
@@ -1,27 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\disk-archive\disk-archive-data\xls\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="25440" windowHeight="12585"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="75">
   <si>
     <t>Мигель де Сервантес Сааведра</t>
   </si>
@@ -237,6 +232,15 @@
   </si>
   <si>
     <t>Номер последнего тома в году</t>
+  </si>
+  <si>
+    <t>Жюль Верн</t>
+  </si>
+  <si>
+    <t>Майн Рид</t>
+  </si>
+  <si>
+    <t>Антон Павлович Чехов</t>
   </si>
 </sst>
 </file>
@@ -277,7 +281,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -293,9 +297,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -333,9 +337,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -370,7 +374,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -405,7 +409,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -579,10 +583,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H179"/>
+  <dimension ref="A1:H203"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+    <sheetView tabSelected="1" topLeftCell="A170" workbookViewId="0">
+      <selection activeCell="B204" sqref="B204"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3658,6 +3662,414 @@
       </c>
       <c r="E179">
         <v>1988</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>72</v>
+      </c>
+      <c r="B180" t="s">
+        <v>29</v>
+      </c>
+      <c r="C180">
+        <v>1</v>
+      </c>
+      <c r="D180">
+        <v>8</v>
+      </c>
+      <c r="E180">
+        <v>1985</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>72</v>
+      </c>
+      <c r="B181" t="s">
+        <v>29</v>
+      </c>
+      <c r="C181">
+        <v>2</v>
+      </c>
+      <c r="D181">
+        <v>8</v>
+      </c>
+      <c r="E181">
+        <v>1985</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>72</v>
+      </c>
+      <c r="B182" t="s">
+        <v>29</v>
+      </c>
+      <c r="C182">
+        <v>3</v>
+      </c>
+      <c r="D182">
+        <v>8</v>
+      </c>
+      <c r="E182">
+        <v>1985</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>72</v>
+      </c>
+      <c r="B183" t="s">
+        <v>29</v>
+      </c>
+      <c r="C183">
+        <v>4</v>
+      </c>
+      <c r="D183">
+        <v>8</v>
+      </c>
+      <c r="E183">
+        <v>1985</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>72</v>
+      </c>
+      <c r="B184" t="s">
+        <v>29</v>
+      </c>
+      <c r="C184">
+        <v>5</v>
+      </c>
+      <c r="D184">
+        <v>8</v>
+      </c>
+      <c r="E184">
+        <v>1985</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>72</v>
+      </c>
+      <c r="B185" t="s">
+        <v>29</v>
+      </c>
+      <c r="C185">
+        <v>6</v>
+      </c>
+      <c r="D185">
+        <v>8</v>
+      </c>
+      <c r="E185">
+        <v>1985</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>72</v>
+      </c>
+      <c r="B186" t="s">
+        <v>29</v>
+      </c>
+      <c r="C186">
+        <v>7</v>
+      </c>
+      <c r="D186">
+        <v>8</v>
+      </c>
+      <c r="E186">
+        <v>1985</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>72</v>
+      </c>
+      <c r="B187" t="s">
+        <v>29</v>
+      </c>
+      <c r="C187">
+        <v>8</v>
+      </c>
+      <c r="D187">
+        <v>8</v>
+      </c>
+      <c r="E187">
+        <v>1985</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>73</v>
+      </c>
+      <c r="B188" t="s">
+        <v>31</v>
+      </c>
+      <c r="C188">
+        <v>1</v>
+      </c>
+      <c r="D188">
+        <v>8</v>
+      </c>
+      <c r="E188">
+        <v>1992</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>73</v>
+      </c>
+      <c r="B189" t="s">
+        <v>31</v>
+      </c>
+      <c r="C189">
+        <v>2</v>
+      </c>
+      <c r="D189">
+        <v>8</v>
+      </c>
+      <c r="E189">
+        <v>1992</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>73</v>
+      </c>
+      <c r="B190" t="s">
+        <v>31</v>
+      </c>
+      <c r="C190">
+        <v>3</v>
+      </c>
+      <c r="D190">
+        <v>8</v>
+      </c>
+      <c r="E190">
+        <v>1992</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>73</v>
+      </c>
+      <c r="B191" t="s">
+        <v>31</v>
+      </c>
+      <c r="C191">
+        <v>4</v>
+      </c>
+      <c r="D191">
+        <v>8</v>
+      </c>
+      <c r="E191">
+        <v>1992</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>73</v>
+      </c>
+      <c r="B192" t="s">
+        <v>31</v>
+      </c>
+      <c r="C192">
+        <v>5</v>
+      </c>
+      <c r="D192">
+        <v>8</v>
+      </c>
+      <c r="E192">
+        <v>1992</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>73</v>
+      </c>
+      <c r="B193" t="s">
+        <v>31</v>
+      </c>
+      <c r="C193">
+        <v>6</v>
+      </c>
+      <c r="D193">
+        <v>8</v>
+      </c>
+      <c r="E193">
+        <v>1992</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>73</v>
+      </c>
+      <c r="B194" t="s">
+        <v>31</v>
+      </c>
+      <c r="C194">
+        <v>7</v>
+      </c>
+      <c r="D194">
+        <v>8</v>
+      </c>
+      <c r="E194">
+        <v>1992</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>73</v>
+      </c>
+      <c r="B195" t="s">
+        <v>31</v>
+      </c>
+      <c r="C195">
+        <v>8</v>
+      </c>
+      <c r="D195">
+        <v>8</v>
+      </c>
+      <c r="E195">
+        <v>1992</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>74</v>
+      </c>
+      <c r="B196" t="s">
+        <v>29</v>
+      </c>
+      <c r="C196">
+        <v>1</v>
+      </c>
+      <c r="D196">
+        <v>8</v>
+      </c>
+      <c r="E196">
+        <v>1970</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>74</v>
+      </c>
+      <c r="B197" t="s">
+        <v>29</v>
+      </c>
+      <c r="C197">
+        <v>2</v>
+      </c>
+      <c r="D197">
+        <v>8</v>
+      </c>
+      <c r="E197">
+        <v>1970</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>74</v>
+      </c>
+      <c r="B198" t="s">
+        <v>29</v>
+      </c>
+      <c r="C198">
+        <v>3</v>
+      </c>
+      <c r="D198">
+        <v>8</v>
+      </c>
+      <c r="E198">
+        <v>1970</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>74</v>
+      </c>
+      <c r="B199" t="s">
+        <v>29</v>
+      </c>
+      <c r="C199">
+        <v>4</v>
+      </c>
+      <c r="D199">
+        <v>8</v>
+      </c>
+      <c r="E199">
+        <v>1970</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>74</v>
+      </c>
+      <c r="B200" t="s">
+        <v>29</v>
+      </c>
+      <c r="C200">
+        <v>5</v>
+      </c>
+      <c r="D200">
+        <v>8</v>
+      </c>
+      <c r="E200">
+        <v>1970</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>74</v>
+      </c>
+      <c r="B201" t="s">
+        <v>29</v>
+      </c>
+      <c r="C201">
+        <v>6</v>
+      </c>
+      <c r="D201">
+        <v>8</v>
+      </c>
+      <c r="E201">
+        <v>1970</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>74</v>
+      </c>
+      <c r="B202" t="s">
+        <v>29</v>
+      </c>
+      <c r="C202">
+        <v>7</v>
+      </c>
+      <c r="D202">
+        <v>8</v>
+      </c>
+      <c r="E202">
+        <v>1970</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>74</v>
+      </c>
+      <c r="B203" t="s">
+        <v>29</v>
+      </c>
+      <c r="C203">
+        <v>8</v>
+      </c>
+      <c r="D203">
+        <v>8</v>
+      </c>
+      <c r="E203">
+        <v>1970</v>
       </c>
     </row>
   </sheetData>

</xml_diff>